<commit_message>
Improve: add E2E test for changing link elements.
</commit_message>
<xml_diff>
--- a/E2ETest/memo.xlsx
+++ b/E2ETest/memo.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\Blazor\HeadElement\E2ETest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AA7F5E8-F7D8-463E-BEDE-AF2A10DB1C3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECC9246A-E229-4BE1-A6F8-4D88427DEEB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6795" yWindow="2250" windowWidth="13500" windowHeight="9360" xr2:uid="{C48BDBF7-6F48-4384-A27E-A37DABAF0DE2}"/>
+    <workbookView xWindow="6900" yWindow="2865" windowWidth="14700" windowHeight="9360" activeTab="1" xr2:uid="{C48BDBF7-6F48-4384-A27E-A37DABAF0DE2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="58">
   <si>
     <t>Home</t>
   </si>
@@ -180,13 +181,45 @@
   </si>
   <si>
     <t>value-H4-C</t>
+  </si>
+  <si>
+    <t>rel=icon</t>
+  </si>
+  <si>
+    <t>rel=stylesheet</t>
+  </si>
+  <si>
+    <t>rel=canonical</t>
+  </si>
+  <si>
+    <t>href=iconA.png</t>
+  </si>
+  <si>
+    <t>href=/counter
+title=link-B</t>
+  </si>
+  <si>
+    <t>href=iconB.png
+type=image/png</t>
+  </si>
+  <si>
+    <t>href=customC.css
+media=print</t>
+  </si>
+  <si>
+    <t>href=/fetchdata
+title=link-C</t>
+  </si>
+  <si>
+    <t>href=customA.css
+title=custom</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -203,6 +236,13 @@
     <font>
       <sz val="11"/>
       <color theme="0" tint="-0.34998626667073579"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -234,13 +274,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -557,8 +603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00A7472A-100C-4F5B-9633-8539990C8251}">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -908,4 +954,117 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0EB9C57-3424-4BC9-AF30-3514FEE2109B}">
+  <dimension ref="B1:I5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="4"/>
+    <col min="2" max="2" width="19.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="5.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="4"/>
+    <col min="7" max="7" width="5.140625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" style="4" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B3" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B4" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
E2E Test - improve performance and implements.
</commit_message>
<xml_diff>
--- a/E2ETest/memo.xlsx
+++ b/E2ETest/memo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\Blazor\HeadElement\E2ETest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECC9246A-E229-4BE1-A6F8-4D88427DEEB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81C02629-03EC-46D9-A42F-42209A820FAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6900" yWindow="2865" windowWidth="14700" windowHeight="9360" activeTab="1" xr2:uid="{C48BDBF7-6F48-4384-A27E-A37DABAF0DE2}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="1" xr2:uid="{C48BDBF7-6F48-4384-A27E-A37DABAF0DE2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="67">
   <si>
     <t>Home</t>
   </si>
@@ -213,6 +213,37 @@
   <si>
     <t>href=customA.css
 title=custom</t>
+  </si>
+  <si>
+    <t>rel=preload</t>
+  </si>
+  <si>
+    <t>href=customX.css</t>
+  </si>
+  <si>
+    <t>href=orange.png</t>
+  </si>
+  <si>
+    <t>href=green.png</t>
+  </si>
+  <si>
+    <t>href=blue.png
+media=min:301px</t>
+  </si>
+  <si>
+    <t>href=red.png
+media=min:601px</t>
+  </si>
+  <si>
+    <t>href=red.png
+media=max:600px</t>
+  </si>
+  <si>
+    <t>href=red.png
+media=min:599px</t>
+  </si>
+  <si>
+    <t>href=purple.png</t>
   </si>
 </sst>
 </file>
@@ -274,7 +305,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -286,6 +317,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -607,20 +644,20 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" customWidth="1"/>
+    <col min="1" max="1" width="17.59765625" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" customWidth="1"/>
-    <col min="4" max="4" width="3.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" customWidth="1"/>
-    <col min="7" max="7" width="3.85546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" customWidth="1"/>
+    <col min="3" max="3" width="12.1328125" customWidth="1"/>
+    <col min="4" max="4" width="3.86328125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.86328125" customWidth="1"/>
+    <col min="6" max="6" width="11.265625" customWidth="1"/>
+    <col min="7" max="7" width="3.86328125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10.86328125" customWidth="1"/>
+    <col min="9" max="9" width="11.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="C1" t="s">
         <v>0</v>
       </c>
@@ -631,7 +668,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -660,7 +697,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
         <v>9</v>
       </c>
@@ -680,7 +717,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
         <v>10</v>
       </c>
@@ -700,7 +737,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
         <v>11</v>
       </c>
@@ -720,7 +757,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
         <v>15</v>
       </c>
@@ -737,7 +774,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -766,7 +803,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
         <v>25</v>
       </c>
@@ -786,7 +823,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B10" t="s">
         <v>26</v>
       </c>
@@ -806,7 +843,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B11" t="s">
         <v>27</v>
       </c>
@@ -826,7 +863,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B12" t="s">
         <v>28</v>
       </c>
@@ -843,7 +880,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>36</v>
       </c>
@@ -872,7 +909,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B15" t="s">
         <v>38</v>
       </c>
@@ -892,7 +929,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B16" t="s">
         <v>39</v>
       </c>
@@ -912,7 +949,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B17" t="s">
         <v>40</v>
       </c>
@@ -932,7 +969,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B18" t="s">
         <v>41</v>
       </c>
@@ -958,24 +995,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0EB9C57-3424-4BC9-AF30-3514FEE2109B}">
-  <dimension ref="B1:I5"/>
+  <dimension ref="B1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="4"/>
-    <col min="2" max="2" width="19.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.140625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="5.7109375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="4"/>
-    <col min="7" max="7" width="5.140625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="17.85546875" style="4" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="9.1328125" style="4"/>
+    <col min="2" max="2" width="19.1328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.1328125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="5.73046875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="16.3984375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="9.1328125" style="7"/>
+    <col min="7" max="7" width="5.1328125" style="4" customWidth="1"/>
+    <col min="8" max="8" width="17.86328125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="9.1328125" style="7"/>
+    <col min="10" max="16384" width="9.1328125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:9" x14ac:dyDescent="0.45">
       <c r="C1" s="4" t="s">
         <v>0</v>
       </c>
@@ -986,7 +1024,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B2" s="4" t="s">
         <v>49</v>
       </c>
@@ -996,71 +1034,206 @@
       <c r="E2" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" s="4" t="s">
+      <c r="H2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B3" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="5" t="s">
+      <c r="C3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>12</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B4" s="4" t="s">
         <v>50</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="4" t="s">
+      <c r="E4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="7" t="s">
         <v>13</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B5" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="6" t="s">
         <v>12</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="7" t="s">
         <v>7</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="I5" s="7" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B7" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B8" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B9" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B10" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B11" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I11" s="4"/>
+    </row>
+    <row r="12" spans="2:9" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B12" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I12" s="4"/>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B13" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B14" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>